<commit_message>
progress on experiments - images with performance
</commit_message>
<xml_diff>
--- a/2019_neurips_vigil/results/Results paper VIGIL_v14.xlsx
+++ b/2019_neurips_vigil/results/Results paper VIGIL_v14.xlsx
@@ -5,17 +5,21 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jayram/research/Topic/Machine Intelligence/VQA/COG_publications/2019_neurips_vigil/results/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tomaszkornuta/Documents/GitHub/COG_publications/2019_neurips_vigil/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3D9F944-D71D-024E-816C-213B3B7701EA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD8C40D6-5C43-CD49-82C7-3C85A4E80880}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19160" activeTab="1" xr2:uid="{3D9B9DCB-639E-0F40-9945-E2955BC58740}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16540" activeTab="1" xr2:uid="{3D9B9DCB-639E-0F40-9945-E2955BC58740}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$D$15:$D$37</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$D$15:$D$37</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -451,6 +455,3491 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>SAMNet</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="bg1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="inEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$15:$A$37</c:f>
+              <c:strCache>
+                <c:ptCount val="23"/>
+                <c:pt idx="0">
+                  <c:v>AndCompareColor</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>AndCompareShape</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>AndSimpleCompareColor</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>AndSimpleCompareShape</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>CompareColor</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>CompareShape</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Exist</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>ExistColor</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>ExistColorOf</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>ExistColorSpace</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>ExistLastColorSameShape</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>ExistLastObjectSameObject</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>ExistLastShapeSameColor</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>ExistShape</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>ExistShapeOf</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>ExistShapeSpace</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>ExistSpace</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>GetColor</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>GetColorSpace</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>GetShape</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>GetShapeSpace</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>SimpleCompareShape</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>SimpleCompareColor</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$15:$D$37</c:f>
+              <c:numCache>
+                <c:formatCode>0.0%</c:formatCode>
+                <c:ptCount val="23"/>
+                <c:pt idx="0">
+                  <c:v>0.93489399939999995</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.93200639259999996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.99196963739999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.99248780709999995</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.98118233160000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.9804640107</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.99971400919999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.99975800770000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.99945901449999996</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.94067396640000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.9945441746</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.97268610249999998</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.98160858849999999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.99402324819999999</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.93500411809999995</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.95311949240000005</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.99988277219999999</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.97992283869999997</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.99990595540000005</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.97484548670000004</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.99938934170000004</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.99981246629999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3241-164C-AAB8-41356EFCC889}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>COG</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="bg1">
+                <a:lumMod val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="bg1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="inEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$T$15:$T$37</c:f>
+              <c:numCache>
+                <c:formatCode>0.0%</c:formatCode>
+                <c:ptCount val="23"/>
+                <c:pt idx="0">
+                  <c:v>0.81871342659000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.79989439249000005</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.99659228324899995</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.99206250906000004</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.99404764175399996</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.98958331346499995</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.99691176414500005</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.98882681131399996</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.98016309738200003</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.98378378152799995</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.98863637447399999</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.98170733451799996</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.98113209009199998</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-3241-164C-AAB8-41356EFCC889}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="20"/>
+        <c:axId val="1113063551"/>
+        <c:axId val="1238457167"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1113063551"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="4500000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1238457167"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="0"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1238457167"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+          <c:min val="0.70000000000000007"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.0%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1113063551"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>SAMNet</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="bg1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="inEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$15:$A$37</c:f>
+              <c:strCache>
+                <c:ptCount val="23"/>
+                <c:pt idx="0">
+                  <c:v>AndCompareColor</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>AndCompareShape</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>AndSimpleCompareColor</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>AndSimpleCompareShape</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>CompareColor</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>CompareShape</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Exist</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>ExistColor</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>ExistColorOf</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>ExistColorSpace</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>ExistLastColorSameShape</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>ExistLastObjectSameObject</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>ExistLastShapeSameColor</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>ExistShape</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>ExistShapeOf</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>ExistShapeSpace</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>ExistSpace</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>GetColor</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>GetColorSpace</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>GetShape</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>GetShapeSpace</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>SimpleCompareShape</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>SimpleCompareColor</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$P$15:$P$37</c:f>
+              <c:numCache>
+                <c:formatCode>0.0%</c:formatCode>
+                <c:ptCount val="23"/>
+                <c:pt idx="0">
+                  <c:v>0.80625043230000004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.80084048129999996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.99428281460000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.99219719009999996</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.99653427920000004</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.99208289670000005</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.99847104890000005</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.99882303770000003</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.99831557859999998</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.90776715659999996</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.97976064770000004</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.97531038370000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.97492080250000002</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.99978000700000003</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.99240861270000003</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.90513366179999999</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.93313131999999999</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.99980693229999995</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.95388314500000004</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.9992844568</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.94336381000000002</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.9988642043</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.99874093990000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-801E-744E-B642-155FD0C3C8AF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>COG</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="bg1">
+                <a:lumMod val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="bg1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="inEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$W$15:$W$37</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="23"/>
+                <c:pt idx="0">
+                  <c:v>0.51400000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.50700000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.78200000000000003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.77900000000000003</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.501</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.505</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.99299999999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.89800000000000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.73099999999999998</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.89200000000000002</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.504</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.60199999999999998</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.503</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.92500000000000004</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.72699999999999998</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.89800000000000002</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.92800000000000005</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.97899999999999998</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.92300000000000004</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.97099999999999997</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.90300000000000002</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.99299999999999999</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.99299999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-801E-744E-B642-155FD0C3C8AF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="20"/>
+        <c:axId val="1113063551"/>
+        <c:axId val="1238457167"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1113063551"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="4500000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1238457167"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="0"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1238457167"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+          <c:min val="0.2"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.0%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1113063551"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>SAMNet</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="5400000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="bg1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="inEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$15:$A$37</c:f>
+              <c:strCache>
+                <c:ptCount val="23"/>
+                <c:pt idx="0">
+                  <c:v>AndCompareColor</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>AndCompareShape</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>AndSimpleCompareColor</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>AndSimpleCompareShape</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>CompareColor</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>CompareShape</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Exist</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>ExistColor</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>ExistColorOf</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>ExistColorSpace</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>ExistLastColorSameShape</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>ExistLastObjectSameObject</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>ExistLastShapeSameColor</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>ExistShape</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>ExistShapeOf</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>ExistShapeSpace</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>ExistSpace</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>GetColor</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>GetColorSpace</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>GetShape</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>GetShapeSpace</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>SimpleCompareShape</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>SimpleCompareColor</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$P$15:$P$37</c:f>
+              <c:numCache>
+                <c:formatCode>0.0%</c:formatCode>
+                <c:ptCount val="23"/>
+                <c:pt idx="0">
+                  <c:v>0.80625043230000004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.80084048129999996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.99428281460000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.99219719009999996</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.99653427920000004</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.99208289670000005</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.99847104890000005</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.99882303770000003</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.99831557859999998</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.90776715659999996</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.97976064770000004</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.97531038370000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.97492080250000002</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.99978000700000003</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.99240861270000003</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.90513366179999999</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.93313131999999999</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.99980693229999995</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.95388314500000004</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.9992844568</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.94336381000000002</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.9988642043</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.99874093990000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-156F-0047-AFEE-0F86259CAF4E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>COG</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="bg1">
+                <a:lumMod val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="5400000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="bg1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="inEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$W$15:$W$37</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="23"/>
+                <c:pt idx="0">
+                  <c:v>0.51400000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.50700000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.78200000000000003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.77900000000000003</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.501</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.505</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.99299999999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.89800000000000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.73099999999999998</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.89200000000000002</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.504</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.60199999999999998</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.503</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.92500000000000004</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.72699999999999998</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.89800000000000002</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.92800000000000005</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.97899999999999998</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.92300000000000004</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.97099999999999997</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.90300000000000002</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.99299999999999999</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.99299999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-156F-0047-AFEE-0F86259CAF4E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="20"/>
+        <c:axId val="1113063551"/>
+        <c:axId val="1238457167"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1113063551"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="4500000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1238457167"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="0"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1238457167"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+          <c:min val="0.2"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.0%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1113063551"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>548408</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>66963</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BB2D0B8D-A143-A849-AEF4-4F107AEA7AC2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>531092</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>150091</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>191655</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2E1E94B8-6E20-454A-8BD2-65194604A746}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>294411</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>41564</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{63F4725A-29E7-9B44-B2B7-6B1AE174AFA5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -3107,6 +6596,13 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="N3:Q3"/>
+    <mergeCell ref="B1:Q1"/>
+    <mergeCell ref="T1:W1"/>
+    <mergeCell ref="Y1:AA1"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="N2:Q2"/>
     <mergeCell ref="K8:L8"/>
     <mergeCell ref="N8:Q8"/>
     <mergeCell ref="K4:L4"/>
@@ -3116,13 +6612,6 @@
     <mergeCell ref="N6:Q6"/>
     <mergeCell ref="K7:L7"/>
     <mergeCell ref="N7:Q7"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="N3:Q3"/>
-    <mergeCell ref="B1:Q1"/>
-    <mergeCell ref="T1:W1"/>
-    <mergeCell ref="Y1:AA1"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="N2:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3132,8 +6621,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F950B3BD-F67F-7347-9596-8AB8CAAAC726}">
   <dimension ref="A1:AD60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="P10" sqref="P10"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="P63" sqref="P63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -5543,5 +9032,6 @@
     <mergeCell ref="L6:Q6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>